<commit_message>
second version: spreadsheet contains list of keywords and weights
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -183,10 +183,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -462,6 +462,90 @@
       <c r="E20" s="1" t="n">
         <v>4</v>
       </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>